<commit_message>
Pull new files from local to repo
</commit_message>
<xml_diff>
--- a/109215_31001.xlsx
+++ b/109215_31001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSc Computer Science - SNUT\Capstone Project\Ares\AutoAttendance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSc Computer Science - SNUT\Capstone Project\Capstone_AttendanceManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF26EA14-480C-4A44-8CEC-0DA7554EB73F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48C3F50-4419-4745-A787-A75DDDBCAC19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>학번</t>
   </si>
@@ -34,46 +34,58 @@
     <t>출석시간</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>15102993</t>
+  </si>
+  <si>
+    <t>16101384</t>
+  </si>
+  <si>
     <t>16101883</t>
   </si>
   <si>
-    <t>16101384</t>
+    <t>17101222</t>
+  </si>
+  <si>
+    <t>18101255</t>
   </si>
   <si>
     <t>18102231</t>
   </si>
   <si>
-    <t>15102993</t>
+    <t>19102395</t>
   </si>
   <si>
     <t>20101023</t>
   </si>
   <si>
-    <t>20101134</t>
-  </si>
-  <si>
-    <t>19102395</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>17101222</t>
-  </si>
-  <si>
-    <t>18101255</t>
+    <t>20101135</t>
+  </si>
+  <si>
+    <t>강동완</t>
+  </si>
+  <si>
+    <t>Ngoc Anh</t>
+  </si>
+  <si>
+    <t>응웬민뚜</t>
   </si>
   <si>
     <t>Khanh Ngan</t>
   </si>
   <si>
-    <t>응웬민뚜</t>
+    <t>안홍현</t>
+  </si>
+  <si>
+    <t>Linh</t>
   </si>
   <si>
     <t>Thanh Danh</t>
   </si>
   <si>
-    <t>Ngoc Anh</t>
+    <t>Anh Duc</t>
   </si>
   <si>
     <t>Nhim</t>
@@ -82,31 +94,22 @@
     <t>Pham Duy Thai</t>
   </si>
   <si>
-    <t>Anh Duc</t>
-  </si>
-  <si>
-    <t>강동완</t>
-  </si>
-  <si>
-    <t>안홍현</t>
-  </si>
-  <si>
-    <t>Linh</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>2020/12/28 21:30:05</t>
-  </si>
-  <si>
-    <t>2020/12/28 21:30:12</t>
-  </si>
-  <si>
-    <t>2020/12/28 21:30:25</t>
-  </si>
-  <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>2020/12/29 00:37:01</t>
+  </si>
+  <si>
+    <t>2020/12/29 00:36:08</t>
+  </si>
+  <si>
+    <t>2020/12/29 00:36:16</t>
+  </si>
+  <si>
+    <t>2020/12/29 00:36:18</t>
   </si>
 </sst>
 </file>
@@ -510,13 +513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -551,11 +557,8 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,6 +568,9 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
@@ -577,7 +583,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -588,7 +594,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -599,7 +605,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -624,7 +630,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -634,8 +640,11 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -649,7 +658,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>